<commit_message>
Fan controllers, vias controlled. slight layout changes for new connectors. removed 5v and ground from hall effects
</commit_message>
<xml_diff>
--- a/2023/Power_and_motor_control/power_and_motor_control/Project Outputs for Free Documents/BOM/Bill of Materials-power_and_motor_control.xlsx
+++ b/2023/Power_and_motor_control/power_and_motor_control/Project Outputs for Free Documents/BOM/Bill of Materials-power_and_motor_control.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elija\Documents\GitHub\PCB\2023\Power_and_motor_control\power_and_motor_control\Project Outputs for Free Documents\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C48FFAD-C3DD-4BE4-86D3-29A085816921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{721135E1-AACE-400F-921A-4BA1569909F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="23040" windowHeight="12204" xr2:uid="{DFE55EDE-A245-4846-BEE5-BFC169A117AF}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="23040" windowHeight="12204" xr2:uid="{062E69EB-5D4E-4ED3-A0A3-CEAAD4705055}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-power_and_mot" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="118">
   <si>
     <t>Comment</t>
   </si>
@@ -59,13 +59,28 @@
     <t>Quantity</t>
   </si>
   <si>
+    <t>Solder Pads</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Battery, Sol1, Sol2, Sol3, Sol4</t>
+  </si>
+  <si>
+    <t>Solder Pad</t>
+  </si>
+  <si>
+    <t>Component_1</t>
+  </si>
+  <si>
     <t>ECA1HM101</t>
   </si>
   <si>
     <t>Aluminum Electrolytic Capacitor, 100 uF, +/- 20%, 50 V, -40 to 85 degC, 2-Pin THD, RoHS, Bulk</t>
   </si>
   <si>
-    <t>C1, C6</t>
+    <t>C1, C6, C24, C25</t>
   </si>
   <si>
     <t>CAPPR65-350-1150X800X1250</t>
@@ -161,13 +176,55 @@
     <t>CMP-06035-010759-1</t>
   </si>
   <si>
+    <t>EEUFM1V331B</t>
+  </si>
+  <si>
+    <t>Aluminum Electrolytic Capacitors (Radial Lead Type) 330uF ±20% 35V</t>
+  </si>
+  <si>
+    <t>C22, C23</t>
+  </si>
+  <si>
+    <t>FP-RAD-TH-D_10_0_5-L_16_1-MFG</t>
+  </si>
+  <si>
+    <t>CMP-05427-002072-1</t>
+  </si>
+  <si>
+    <t>19R472C</t>
+  </si>
+  <si>
+    <t>No Description Available</t>
+  </si>
+  <si>
+    <t>L1, L2, L3, L4, L5, L6</t>
+  </si>
+  <si>
+    <t>1900R_MUR</t>
+  </si>
+  <si>
+    <t>B5B-XH-AM(LF)(SN)</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 5POS 2.5MM</t>
+  </si>
+  <si>
+    <t>P_hall_in, S_hall_in</t>
+  </si>
+  <si>
+    <t>FP-B5B-XH-AM_LF_SN-MFG</t>
+  </si>
+  <si>
+    <t>CMP-17439-000304-1</t>
+  </si>
+  <si>
     <t>B3B-XH-A(LF)(SN)</t>
   </si>
   <si>
     <t>CONN HEADER VERT 3POS 2.5MM</t>
   </si>
   <si>
-    <t>J1, J16, J17</t>
+    <t>P_in, S_in, Sol_in</t>
   </si>
   <si>
     <t>FP-B3B-XH-A_LF_SN-MFG</t>
@@ -176,139 +233,166 @@
     <t>CMP-17439-000014-3</t>
   </si>
   <si>
+    <t>Single Solder Pad</t>
+  </si>
+  <si>
+    <t>Pmot1, Pmot2, Pmot3, Smot1, Smot2, Smot3</t>
+  </si>
+  <si>
+    <t>SOLDER PAD SINGLE</t>
+  </si>
+  <si>
+    <t>singlesolpad_1</t>
+  </si>
+  <si>
+    <t>I7C4W012A050V-001-R</t>
+  </si>
+  <si>
+    <t>Non-Isolated PoL Module DC DC Converter 1 Output 5 ~ 28V - - - 12.5A 9V - 53V Input</t>
+  </si>
+  <si>
+    <t>PS1</t>
+  </si>
+  <si>
+    <t>CONV_I7C4W012A050V-001-R</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>RES 1.05K OHM 0.5% 1/5W 0805   MCU08050D1002BP100</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4</t>
+  </si>
+  <si>
+    <t>FP-MCU0805-IPC_C</t>
+  </si>
+  <si>
+    <t>CMP-02407-010458-1</t>
+  </si>
+  <si>
+    <t>MCU08050D1002BP100</t>
+  </si>
+  <si>
+    <t>RES 1.05K OHM 0.5% 1/5W 0805</t>
+  </si>
+  <si>
+    <t>R5, R7</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>Thick Film Chip Resistors 0805 100kΩ 0.125W 5% 200ppm/°C CR0805-JW-104GLF</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>FP-CR0805-MFG</t>
+  </si>
+  <si>
+    <t>CMP-07231-001707-1</t>
+  </si>
+  <si>
+    <t>7.5k</t>
+  </si>
+  <si>
+    <t>ERJ-6GEYJ752V</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>RESC2013X70X40LL20T20</t>
+  </si>
+  <si>
+    <t>CMP-2001-00447-1</t>
+  </si>
+  <si>
+    <t>CRCW0805560KFKEA</t>
+  </si>
+  <si>
+    <t>RES Thick Film, 560kΩ, 1%, 0.125W, 100ppm/°C, 0805</t>
+  </si>
+  <si>
+    <t>Rtrim</t>
+  </si>
+  <si>
+    <t>FP-CRCW0805-e3-IPC_A</t>
+  </si>
+  <si>
+    <t>CMP-2001-04009-2</t>
+  </si>
+  <si>
+    <t>Screw M3</t>
+  </si>
+  <si>
+    <t>S1, S2, S3, S4</t>
+  </si>
+  <si>
+    <t>MS12ANW03</t>
+  </si>
+  <si>
+    <t>Slide Switch SPDT Through Hole</t>
+  </si>
+  <si>
+    <t>S21, S23</t>
+  </si>
+  <si>
+    <t>SW_MS12ANW03</t>
+  </si>
+  <si>
+    <t>MP6610GS-P</t>
+  </si>
+  <si>
+    <t>U1, U2, U3, U4</t>
+  </si>
+  <si>
+    <t>SOIC-8_MP6610_MNP</t>
+  </si>
+  <si>
+    <t>U5, U6</t>
+  </si>
+  <si>
+    <t>Motor_Driver</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>5v_supply</t>
+  </si>
+  <si>
+    <t>LM1117T-3.3/NOPB</t>
+  </si>
+  <si>
+    <t>800mA Low-Dropout Linear Regulator, 3-pin TO-220, Pb-Free</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>NDE0003A</t>
+  </si>
+  <si>
+    <t>CMP-0062-02494-3</t>
+  </si>
+  <si>
     <t>B2B-XH-A(LF)(SN)</t>
   </si>
   <si>
     <t>CONN HEADER VERT 2POS 2.5MM</t>
   </si>
   <si>
-    <t>J2, J3, J6</t>
+    <t>V_sense</t>
   </si>
   <si>
     <t>FP-B2B-XH-A_LF_SN-MFG</t>
   </si>
   <si>
     <t>CMP-2000-05888-3</t>
-  </si>
-  <si>
-    <t>Solder Pads</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>J4, J5, J7, J8, J9, J10, J11, J12, J13, J14, J15</t>
-  </si>
-  <si>
-    <t>Solder Pad</t>
-  </si>
-  <si>
-    <t>Component_1</t>
-  </si>
-  <si>
-    <t>19R472C</t>
-  </si>
-  <si>
-    <t>No Description Available</t>
-  </si>
-  <si>
-    <t>L1, L2, L3, L4, L5, L6</t>
-  </si>
-  <si>
-    <t>1900R_MUR</t>
-  </si>
-  <si>
-    <t>I7C4W012A050V-001-R</t>
-  </si>
-  <si>
-    <t>Non-Isolated PoL Module DC DC Converter 1 Output 5 ~ 28V - - - 12.5A 9V - 53V Input</t>
-  </si>
-  <si>
-    <t>PS1</t>
-  </si>
-  <si>
-    <t>CONV_I7C4W012A050V-001-R</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>RES 1.05K OHM 0.5% 1/5W 0805   MCU08050D1002BP100</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4</t>
-  </si>
-  <si>
-    <t>FP-MCU0805-IPC_C</t>
-  </si>
-  <si>
-    <t>CMP-02407-010458-1</t>
-  </si>
-  <si>
-    <t>MCU08050D1002BP100</t>
-  </si>
-  <si>
-    <t>RES 1.05K OHM 0.5% 1/5W 0805</t>
-  </si>
-  <si>
-    <t>R5, R6, R7, R8</t>
-  </si>
-  <si>
-    <t>Screw M3</t>
-  </si>
-  <si>
-    <t>S1, S2, S3, S4</t>
-  </si>
-  <si>
-    <t>MS12ANW03</t>
-  </si>
-  <si>
-    <t>Slide Switch SPDT Through Hole</t>
-  </si>
-  <si>
-    <t>S21, S23</t>
-  </si>
-  <si>
-    <t>SW_MS12ANW03</t>
-  </si>
-  <si>
-    <t>MP6610GS-P</t>
-  </si>
-  <si>
-    <t>U1, U2, U3, U4</t>
-  </si>
-  <si>
-    <t>SOIC-8_MP6610_MNP</t>
-  </si>
-  <si>
-    <t>U5, U6</t>
-  </si>
-  <si>
-    <t>PCBComponent_1</t>
-  </si>
-  <si>
-    <t>5v Power Supply</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>5v_supply</t>
-  </si>
-  <si>
-    <t>LM1117T-3.3/NOPB</t>
-  </si>
-  <si>
-    <t>800mA Low-Dropout Linear Regulator, 3-pin TO-220, Pb-Free</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>NDE0003A</t>
-  </si>
-  <si>
-    <t>CMP-0062-02494-3</t>
   </si>
 </sst>
 </file>
@@ -684,8 +768,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41176323-6F76-49D9-AF4F-14FF746AD158}">
-  <dimension ref="A1:F21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D8D63B-DA38-4E69-8B2D-6E0D87531257}">
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -731,7 +815,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -751,7 +835,7 @@
         <v>15</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -791,7 +875,7 @@
         <v>25</v>
       </c>
       <c r="F5" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -811,7 +895,7 @@
         <v>30</v>
       </c>
       <c r="F6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -831,7 +915,7 @@
         <v>35</v>
       </c>
       <c r="F7" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -845,33 +929,33 @@
         <v>38</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F8" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>44</v>
       </c>
       <c r="F9" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -891,7 +975,7 @@
         <v>49</v>
       </c>
       <c r="F10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -908,30 +992,30 @@
         <v>53</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F11" s="1">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="F12" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -948,18 +1032,18 @@
         <v>62</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="F13" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>65</v>
@@ -971,7 +1055,7 @@
         <v>67</v>
       </c>
       <c r="F14" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -985,30 +1069,30 @@
         <v>70</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F15" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F16" s="1">
         <v>4</v>
@@ -1016,19 +1100,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="F17" s="1">
         <v>2</v>
@@ -1036,59 +1120,59 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="F18" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="F19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>51</v>
+        <v>91</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="F20" s="1">
         <v>1</v>
@@ -1096,21 +1180,141 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F21" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>